<commit_message>
Atualização das categorias no BD
</commit_message>
<xml_diff>
--- a/data/raw/fluxo-financeiro.xlsx
+++ b/data/raw/fluxo-financeiro.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
-    <sheet name="exemplo" sheetId="5" r:id="rId1"/>
-    <sheet name="categorias" sheetId="1" r:id="rId2"/>
-    <sheet name="fluxo" sheetId="2" r:id="rId3"/>
+    <sheet name="categorias" sheetId="1" r:id="rId1"/>
+    <sheet name="fluxo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Categoria</t>
   </si>
@@ -27,15 +26,9 @@
     <t>Entreterimento</t>
   </si>
   <si>
-    <t>Saude</t>
-  </si>
-  <si>
     <t>Transporte</t>
   </si>
   <si>
-    <t>Restaurante</t>
-  </si>
-  <si>
     <t>Receita</t>
   </si>
   <si>
@@ -51,102 +44,12 @@
     <t>Moradia</t>
   </si>
   <si>
-    <t>Compras</t>
-  </si>
-  <si>
-    <t>Escola</t>
-  </si>
-  <si>
-    <t>Faculdade</t>
-  </si>
-  <si>
-    <t>Roupas</t>
-  </si>
-  <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>Mercado</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>Curso</t>
-  </si>
-  <si>
-    <t>Netflix</t>
-  </si>
-  <si>
     <t>Cinema</t>
   </si>
   <si>
     <t>Viagem</t>
   </si>
   <si>
-    <t>Ação</t>
-  </si>
-  <si>
-    <t>Titulo</t>
-  </si>
-  <si>
-    <t>Aluguel</t>
-  </si>
-  <si>
-    <t>Luz</t>
-  </si>
-  <si>
-    <t>Água</t>
-  </si>
-  <si>
-    <t>Gás</t>
-  </si>
-  <si>
-    <t>IPTU</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Telefone fixo</t>
-  </si>
-  <si>
-    <t>Manutenção</t>
-  </si>
-  <si>
-    <t>Médico</t>
-  </si>
-  <si>
-    <t>Dentista</t>
-  </si>
-  <si>
-    <t>Combustivel</t>
-  </si>
-  <si>
-    <t>Plano de saude</t>
-  </si>
-  <si>
-    <t>Manutenção do carro</t>
-  </si>
-  <si>
-    <t>Pedagio</t>
-  </si>
-  <si>
-    <t>Estacionamento</t>
-  </si>
-  <si>
-    <t>IPVA</t>
-  </si>
-  <si>
-    <t>Passagem de avião</t>
-  </si>
-  <si>
-    <t>Hotel</t>
-  </si>
-  <si>
-    <t>Vale</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -156,31 +59,10 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>Salário</t>
-  </si>
-  <si>
-    <t>Lucro de investimento</t>
-  </si>
-  <si>
-    <t>Fretado</t>
-  </si>
-  <si>
-    <t>Onibus</t>
-  </si>
-  <si>
-    <t>Uber</t>
-  </si>
-  <si>
-    <t>Passeio</t>
-  </si>
-  <si>
-    <t>Show</t>
-  </si>
-  <si>
-    <t>Fundo</t>
-  </si>
-  <si>
-    <t>Plano do celular</t>
+    <t>Diversificados</t>
+  </si>
+  <si>
+    <t>Supermecado</t>
   </si>
 </sst>
 </file>
@@ -251,27 +133,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -301,6 +162,27 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -312,45 +194,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:J10" totalsRowShown="0">
-  <tableColumns count="10">
-    <tableColumn id="1" name="Alimentação"/>
-    <tableColumn id="2" name="Compras"/>
-    <tableColumn id="3" name="Educação"/>
-    <tableColumn id="4" name="Entreterimento"/>
-    <tableColumn id="5" name="Investimentos"/>
-    <tableColumn id="6" name="Moradia"/>
-    <tableColumn id="7" name="Receita"/>
-    <tableColumn id="8" name="Saude"/>
-    <tableColumn id="9" name="Transporte"/>
-    <tableColumn id="10" name="Viagem"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:A11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <sortState ref="A2:A11">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="2" name="Categoria" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:A11" totalsRowShown="0" headerRowDxfId="2" dataDxfId="0">
-  <sortState ref="A2:A11">
-    <sortCondition ref="A2"/>
-  </sortState>
-  <tableColumns count="1">
-    <tableColumn id="2" name="Categoria" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D3" totalsRowShown="0" headerRowDxfId="4">
   <sortState ref="A2:I78">
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Data" dataDxfId="6"/>
-    <tableColumn id="3" name="Categoria" dataDxfId="5"/>
-    <tableColumn id="6" name="Descricao" dataDxfId="4"/>
-    <tableColumn id="7" name="Valor" dataDxfId="3" dataCellStyle="Moeda"/>
+    <tableColumn id="1" name="Data" dataDxfId="3"/>
+    <tableColumn id="3" name="Categoria" dataDxfId="2"/>
+    <tableColumn id="6" name="Descricao" dataDxfId="1"/>
+    <tableColumn id="7" name="Valor" dataDxfId="0" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -643,211 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,7 +535,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -882,7 +545,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -912,32 +575,32 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -951,42 +614,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>44200</v>
+        <v>44384</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>44385</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add dados do cartao Caju
</commit_message>
<xml_diff>
--- a/data/raw/fluxo-financeiro.xlsx
+++ b/data/raw/fluxo-financeiro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="categorias" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="17">
   <si>
     <t>Categoria</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Moradia</t>
   </si>
   <si>
-    <t>Cinema</t>
-  </si>
-  <si>
     <t>Viagem</t>
   </si>
   <si>
@@ -62,7 +59,13 @@
     <t>Diversificados</t>
   </si>
   <si>
-    <t>Supermecado</t>
+    <t>vale empresa</t>
+  </si>
+  <si>
+    <t>combustivel</t>
+  </si>
+  <si>
+    <t>restaurante</t>
   </si>
 </sst>
 </file>
@@ -72,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +95,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -126,6 +134,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -206,7 +215,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D3" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D36" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D36"/>
   <sortState ref="A2:I78">
     <sortCondition ref="A2"/>
   </sortState>
@@ -509,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -545,7 +555,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -600,7 +610,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -616,61 +626,523 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>44384</v>
+        <v>44183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="6">
-        <v>200</v>
+        <v>276.32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <v>44195</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44203</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>44210</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>44215</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44216</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="10">
+        <v>285.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44219</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>44223</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>44227</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="10">
+        <v>151.41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44238</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44247</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44247</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44252</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44254</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44254</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="10">
+        <v>106.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44258</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44263</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44275</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44276</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44280</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44295</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44331</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44336</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>44376</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>44385</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6">
-        <v>50</v>
+      <c r="B36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="10">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -681,18 +1153,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>categorias!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>categorias!$A$2:$A$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3:B1048576</xm:sqref>
+          <xm:sqref>B2:B36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add dados do cartao Nubank
</commit_message>
<xml_diff>
--- a/data/raw/fluxo-financeiro.xlsx
+++ b/data/raw/fluxo-financeiro.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="29">
   <si>
     <t>Categoria</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Receita</t>
   </si>
   <si>
-    <t>Investimentos</t>
-  </si>
-  <si>
     <t>Alimentação</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>Diversificados</t>
-  </si>
-  <si>
     <t>vale empresa</t>
   </si>
   <si>
@@ -66,6 +60,48 @@
   </si>
   <si>
     <t>restaurante</t>
+  </si>
+  <si>
+    <t>Americanas</t>
+  </si>
+  <si>
+    <t>Amazon prime video</t>
+  </si>
+  <si>
+    <t>Ifood</t>
+  </si>
+  <si>
+    <t>Estacionamento</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Mercado livre</t>
+  </si>
+  <si>
+    <t>Beyoung</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>Shopee</t>
+  </si>
+  <si>
+    <t>estacionamento</t>
+  </si>
+  <si>
+    <t>mercado</t>
+  </si>
+  <si>
+    <t>roupa</t>
+  </si>
+  <si>
+    <t>Superfluo</t>
+  </si>
+  <si>
+    <t>Investimento</t>
   </si>
 </sst>
 </file>
@@ -100,6 +136,7 @@
       <sz val="9"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,9 +252,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D36" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D36"/>
-  <sortState ref="A2:I78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D80" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D80"/>
+  <sortState ref="A2:D80">
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="4">
@@ -520,7 +557,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +582,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -555,7 +592,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -565,7 +602,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -575,7 +612,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -585,22 +622,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -610,7 +647,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -626,11 +663,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,475 +680,472 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>44183</v>
+        <v>44163</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D2" s="6">
-        <v>276.32</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>44195</v>
+        <v>44176</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="6">
-        <v>75</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>44203</v>
+        <v>44177</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6">
-        <v>75</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44210</v>
+        <v>44183</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="10">
-        <v>70</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="6">
+        <v>276.32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44215</v>
+        <v>44183</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="10">
-        <v>55</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="6">
+        <v>33.090000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44216</v>
+        <v>44193</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="10">
-        <v>285.32</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="6">
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>44219</v>
+        <v>44194</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="10">
-        <v>100</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>44223</v>
+        <v>44195</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="10">
-        <v>6.16</v>
+        <v>13</v>
+      </c>
+      <c r="D9" s="6">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>44227</v>
+        <v>44200</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="10">
-        <v>151.41</v>
+        <v>26</v>
+      </c>
+      <c r="D10" s="6">
+        <v>50.97</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>44238</v>
+        <v>44201</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="10">
-        <v>41</v>
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>44247</v>
+        <v>44203</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="10">
-        <v>291.48</v>
+        <v>13</v>
+      </c>
+      <c r="D12" s="6">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>44247</v>
+        <v>44208</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="10">
-        <v>80</v>
+        <v>16</v>
+      </c>
+      <c r="D13" s="6">
+        <v>9.9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>44252</v>
+        <v>44210</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" s="10">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>44254</v>
+        <v>44215</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="10">
-        <v>200</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>44254</v>
+        <v>44216</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D16" s="10">
-        <v>106.32</v>
+        <v>285.32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>44258</v>
+        <v>44219</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" s="10">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>44263</v>
+        <v>44221</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="10">
-        <v>80</v>
+        <v>19</v>
+      </c>
+      <c r="D18" s="6">
+        <v>91.42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44275</v>
+        <v>44223</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19" s="10">
-        <v>291.48</v>
+        <v>6.16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44276</v>
+        <v>44224</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="10">
-        <v>100</v>
+        <v>22</v>
+      </c>
+      <c r="D20" s="6">
+        <v>392</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>44280</v>
+        <v>44224</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="10">
-        <v>80</v>
+        <v>26</v>
+      </c>
+      <c r="D21" s="6">
+        <v>50.97</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>44287</v>
+        <v>44227</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22" s="10">
-        <v>80</v>
+        <v>151.41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>44295</v>
+        <v>44227</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="10">
-        <v>90</v>
+        <v>25</v>
+      </c>
+      <c r="D23" s="6">
+        <v>15.32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>44306</v>
+        <v>44237</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="10">
-        <v>291.48</v>
+        <v>18</v>
+      </c>
+      <c r="D24" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>44308</v>
+        <v>44238</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D25" s="10">
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>44317</v>
+        <v>44239</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="10">
-        <v>80</v>
+        <v>16</v>
+      </c>
+      <c r="D26" s="6">
+        <v>9.9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>44321</v>
+        <v>44247</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D27" s="10">
-        <v>80</v>
+        <v>291.48</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>44331</v>
+        <v>44247</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D28" s="10">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>44336</v>
+        <v>44250</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="10">
-        <v>291.48</v>
+        <v>27</v>
+      </c>
+      <c r="D29" s="6">
+        <v>33.909999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>44339</v>
+        <v>44252</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D30" s="10">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>44358</v>
+        <v>44252</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="10">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="D31" s="6">
+        <v>55.8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>44365</v>
+        <v>44254</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D32" s="10">
-        <v>291.48</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>44367</v>
+        <v>44254</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="10">
-        <v>80</v>
+        <v>106.32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>44376</v>
+        <v>44258</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D34" s="10">
         <v>80</v>
@@ -1119,13 +1153,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>44381</v>
+        <v>44263</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D35" s="10">
         <v>80</v>
@@ -1133,16 +1167,632 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
+        <v>44267</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="6">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>44275</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>44276</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>44276</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="6">
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>44279</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="6">
+        <v>75.180000000000007</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>44280</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>44295</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>44298</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="6">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="6">
+        <v>169.85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="6">
+        <v>87.58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>44324</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>44328</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="6">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>44331</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>44336</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>44336</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="6">
+        <v>200.56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>44337</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>44338</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="6">
+        <v>214.62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="6">
+        <v>73.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="6">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="6">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="6">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="6">
+        <v>66.790000000000006</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="6">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>44359</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" s="6">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D69" s="6">
+        <v>34.69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="6">
+        <v>45.76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>44376</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>44382</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D78" s="6">
+        <v>68.69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>44385</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="10">
+      <c r="B79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="10">
         <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>44413</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="6">
+        <v>68.69</v>
       </c>
     </row>
   </sheetData>
@@ -1153,12 +1803,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>categorias!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B36</xm:sqref>
+          <xm:sqref>B2:B80</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add dados cartao itau ate fevereiro
</commit_message>
<xml_diff>
--- a/data/raw/fluxo-financeiro.xlsx
+++ b/data/raw/fluxo-financeiro.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="36">
   <si>
     <t>Categoria</t>
   </si>
@@ -102,6 +102,27 @@
   </si>
   <si>
     <t>Investimento</t>
+  </si>
+  <si>
+    <t>taxa banco</t>
+  </si>
+  <si>
+    <t>salario</t>
+  </si>
+  <si>
+    <t>farmacia</t>
+  </si>
+  <si>
+    <t>Ciranda brinquedos</t>
+  </si>
+  <si>
+    <t>Desconhecido</t>
+  </si>
+  <si>
+    <t>Financeiro</t>
+  </si>
+  <si>
+    <t>transferencia</t>
   </si>
 </sst>
 </file>
@@ -111,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +159,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -172,6 +198,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -240,8 +267,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:A11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <sortState ref="A2:A11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:A13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <sortState ref="A2:A13">
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="1">
@@ -252,8 +279,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D80" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D146" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D146"/>
   <sortState ref="A2:D80">
     <sortCondition ref="A2"/>
   </sortState>
@@ -554,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,7 +619,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -602,7 +629,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -612,7 +639,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -622,31 +649,41 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -663,11 +700,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1795,6 +1832,894 @@
         <v>68.69</v>
       </c>
     </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>44169</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D82" s="6">
+        <v>200.93</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" s="6">
+        <v>8.15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>44172</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>44172</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" s="6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>44181</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D90" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>44183</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D91" s="6">
+        <v>3439.19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>44186</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>44186</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93" s="6">
+        <v>246.64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>44186</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="6">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>44186</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" s="6">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>44193</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" s="6">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>44193</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D97" s="6">
+        <v>291.83999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>44194</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" s="11">
+        <v>59.67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D100" s="11">
+        <v>15.41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="11">
+        <v>32.03</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>44201</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103" s="11">
+        <v>8.15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>44204</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>44207</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>44207</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" s="11">
+        <v>31.23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>44207</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="11">
+        <v>75.3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>44207</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" s="11">
+        <v>103.4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>44210</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D109" s="11">
+        <v>38.25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>44210</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D110" s="11">
+        <v>21.69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D112" s="11">
+        <v>46.9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="11">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" s="11">
+        <v>349.11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>44215</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="11">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>44218</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D116" s="11">
+        <v>42.27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>44218</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D117" s="11">
+        <v>175.4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>44218</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D118" s="11">
+        <v>1096.74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>44221</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="11">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>44221</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="11">
+        <v>392.14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>44221</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D121" s="11">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>44222</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>44222</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D123" s="11">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>44223</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D124" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>44223</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D125" s="11">
+        <v>1873.23</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="11">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D127" s="11">
+        <v>27.47</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
+        <v>44229</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128" s="11">
+        <v>8.15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D130" s="11">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="1">
+        <v>44235</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131" s="11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="1">
+        <v>44235</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D132" s="11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="1">
+        <v>44238</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D133" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="1">
+        <v>44238</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="11">
+        <v>99.01</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="1">
+        <v>44238</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D135" s="11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D136" s="11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D137" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D138" s="11">
+        <v>177.81</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D139" s="11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="1">
+        <v>44246</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D140" s="11">
+        <v>44.07</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="1">
+        <v>44246</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" s="11">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="1">
+        <v>44249</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D142" s="11">
+        <v>10.34</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="1">
+        <v>44249</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D143" s="11">
+        <v>51.29</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="1">
+        <v>44249</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D144" s="11">
+        <v>23.79</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="1">
+        <v>44249</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="1">
+        <v>44253</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D146" s="11">
+        <v>2121.6999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1803,12 +2728,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>categorias!$A$2:$A$11</xm:f>
+            <xm:f>categorias!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B80</xm:sqref>
+          <xm:sqref>B2:B146</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add dados cartao itau ate 14/07
</commit_message>
<xml_diff>
--- a/data/raw/fluxo-financeiro.xlsx
+++ b/data/raw/fluxo-financeiro.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="41">
   <si>
     <t>Categoria</t>
   </si>
@@ -98,9 +98,6 @@
     <t>roupa</t>
   </si>
   <si>
-    <t>Superfluo</t>
-  </si>
-  <si>
     <t>Investimento</t>
   </si>
   <si>
@@ -123,6 +120,24 @@
   </si>
   <si>
     <t>transferencia</t>
+  </si>
+  <si>
+    <t>Gasto pessoal</t>
+  </si>
+  <si>
+    <t>escola</t>
+  </si>
+  <si>
+    <t>Decathlon</t>
+  </si>
+  <si>
+    <t>saque</t>
+  </si>
+  <si>
+    <t>barbearia</t>
+  </si>
+  <si>
+    <t>consulta</t>
   </si>
 </sst>
 </file>
@@ -280,9 +295,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D146" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D146"/>
-  <sortState ref="A2:D80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D232" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D232"/>
+  <sortState ref="A2:D233">
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="4">
@@ -585,7 +600,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A13" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,7 +635,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -650,32 +665,32 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -701,11 +716,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D146"/>
+  <dimension ref="A1:D232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G222" sqref="G222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,91 +761,82 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>44176</v>
+        <v>44167</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D3" s="6">
-        <v>25.2</v>
+        <v>8.15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>44177</v>
+        <v>44168</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6">
-        <v>9.9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44183</v>
+        <v>44169</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6">
-        <v>276.32</v>
+        <v>200.93</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44183</v>
+        <v>44172</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6">
-        <v>33.090000000000003</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44193</v>
+        <v>44172</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D7" s="6">
-        <v>392</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>44194</v>
+        <v>44173</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D8" s="6">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>44195</v>
+        <v>44174</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
@@ -839,359 +845,356 @@
         <v>13</v>
       </c>
       <c r="D9" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>44200</v>
+        <v>44176</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D10" s="6">
-        <v>50.97</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>44201</v>
+        <v>44176</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" s="6">
-        <v>5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>44203</v>
+        <v>44177</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6">
-        <v>75</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>44208</v>
+        <v>44179</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D13" s="6">
-        <v>9.9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>44210</v>
+        <v>44181</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="10">
-        <v>70</v>
+        <v>35</v>
+      </c>
+      <c r="D14" s="6">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>44215</v>
+        <v>44183</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="10">
-        <v>55</v>
+        <v>12</v>
+      </c>
+      <c r="D15" s="6">
+        <v>276.32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>44216</v>
+        <v>44183</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="10">
-        <v>285.32</v>
+        <v>17</v>
+      </c>
+      <c r="D16" s="6">
+        <v>33.090000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>44219</v>
+        <v>44183</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="10">
-        <v>100</v>
+        <v>29</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3439.19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>44221</v>
+        <v>44186</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D18" s="6">
-        <v>91.42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44223</v>
+        <v>44186</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="10">
-        <v>6.16</v>
+        <v>25</v>
+      </c>
+      <c r="D19" s="6">
+        <v>246.64</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44224</v>
+        <v>44186</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D20" s="6">
-        <v>392</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>44224</v>
+        <v>44186</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D21" s="6">
-        <v>50.97</v>
+        <v>48.9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>44227</v>
+        <v>44193</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="10">
-        <v>151.41</v>
+        <v>22</v>
+      </c>
+      <c r="D22" s="6">
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>44227</v>
+        <v>44193</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D23" s="6">
-        <v>15.32</v>
+        <v>48.8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>44237</v>
+        <v>44193</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D24" s="6">
-        <v>5</v>
+        <v>291.83999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>44238</v>
+        <v>44194</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="10">
-        <v>41</v>
+        <v>24</v>
+      </c>
+      <c r="D25" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>44239</v>
+        <v>44194</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6">
-        <v>9.9</v>
+        <v>32</v>
+      </c>
+      <c r="D26" s="11">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>44247</v>
+        <v>44195</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="10">
-        <v>291.48</v>
+        <v>13</v>
+      </c>
+      <c r="D27" s="6">
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>44247</v>
+        <v>44200</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="10">
-        <v>80</v>
+        <v>26</v>
+      </c>
+      <c r="D28" s="6">
+        <v>50.97</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>44250</v>
+        <v>44200</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="6">
-        <v>33.909999999999997</v>
+        <v>35</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="11">
+        <v>59.67</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>44252</v>
+        <v>44200</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="10">
-        <v>80</v>
+        <v>30</v>
+      </c>
+      <c r="D30" s="11">
+        <v>15.41</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>44252</v>
+        <v>44200</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="6">
-        <v>55.8</v>
+        <v>14</v>
+      </c>
+      <c r="D31" s="11">
+        <v>32.03</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>44254</v>
+        <v>44200</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="10">
-        <v>200</v>
+        <v>24</v>
+      </c>
+      <c r="D32" s="11">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>44254</v>
+        <v>44201</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="10">
-        <v>106.32</v>
+        <v>18</v>
+      </c>
+      <c r="D33" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>44258</v>
+        <v>44201</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="10">
-        <v>80</v>
+        <v>28</v>
+      </c>
+      <c r="D34" s="11">
+        <v>8.15</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>44263</v>
+        <v>44203</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>3</v>
@@ -1199,97 +1202,97 @@
       <c r="C35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="10">
-        <v>80</v>
+      <c r="D35" s="6">
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>44267</v>
+        <v>44204</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="6">
-        <v>9.9</v>
+        <v>14</v>
+      </c>
+      <c r="D36" s="11">
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>44275</v>
+        <v>44207</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="10">
-        <v>291.48</v>
+        <v>24</v>
+      </c>
+      <c r="D37" s="11">
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>44276</v>
+        <v>44207</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="10">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="D38" s="11">
+        <v>31.23</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>44276</v>
+        <v>44207</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="6">
-        <v>75.900000000000006</v>
+        <v>14</v>
+      </c>
+      <c r="D39" s="11">
+        <v>75.3</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>44279</v>
+        <v>44207</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="6">
-        <v>75.180000000000007</v>
+        <v>14</v>
+      </c>
+      <c r="D40" s="11">
+        <v>103.4</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>44280</v>
+        <v>44208</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="10">
-        <v>80</v>
+        <v>16</v>
+      </c>
+      <c r="D41" s="6">
+        <v>9.9</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>44287</v>
+        <v>44210</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>3</v>
@@ -1298,180 +1301,180 @@
         <v>13</v>
       </c>
       <c r="D42" s="10">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>44295</v>
+        <v>44210</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="10">
-        <v>90</v>
+        <v>14</v>
+      </c>
+      <c r="D43" s="11">
+        <v>38.25</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>44298</v>
+        <v>44210</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="6">
-        <v>9.9</v>
+        <v>14</v>
+      </c>
+      <c r="D44" s="11">
+        <v>21.69</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>44306</v>
+        <v>44214</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="10">
-        <v>291.48</v>
+        <v>18</v>
+      </c>
+      <c r="D45" s="11">
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>44308</v>
+        <v>44214</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="10">
-        <v>85</v>
+        <v>14</v>
+      </c>
+      <c r="D46" s="11">
+        <v>46.9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>44315</v>
+        <v>44214</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="6">
-        <v>169.85</v>
+        <v>14</v>
+      </c>
+      <c r="D47" s="11">
+        <v>18.5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>44317</v>
+        <v>44214</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="10">
-        <v>80</v>
+        <v>25</v>
+      </c>
+      <c r="D48" s="11">
+        <v>349.11</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>44320</v>
+        <v>44215</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="6">
-        <v>87.58</v>
+        <v>13</v>
+      </c>
+      <c r="D49" s="10">
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>44321</v>
+        <v>44215</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="10">
-        <v>80</v>
+        <v>14</v>
+      </c>
+      <c r="D50" s="11">
+        <v>36.9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>44322</v>
+        <v>44216</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="6">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D51" s="10">
+        <v>285.32</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>44324</v>
+        <v>44218</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="6">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D52" s="11">
+        <v>42.27</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>44328</v>
+        <v>44218</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="6">
-        <v>9.9</v>
+        <v>25</v>
+      </c>
+      <c r="D53" s="11">
+        <v>175.4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>44329</v>
+        <v>44218</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="6">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="D54" s="11">
+        <v>1096.74</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>44331</v>
+        <v>44219</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>3</v>
@@ -1480,166 +1483,160 @@
         <v>13</v>
       </c>
       <c r="D55" s="10">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>44336</v>
+        <v>44221</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="10">
-        <v>291.48</v>
+        <v>19</v>
+      </c>
+      <c r="D56" s="6">
+        <v>91.42</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>44336</v>
+        <v>44221</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="6">
-        <v>200.56</v>
+        <v>14</v>
+      </c>
+      <c r="D57" s="11">
+        <v>23.8</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>44337</v>
+        <v>44221</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="6">
-        <v>130</v>
+        <v>25</v>
+      </c>
+      <c r="D58" s="11">
+        <v>392.14</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>44338</v>
+        <v>44221</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="6">
-        <v>214.62</v>
+        <v>30</v>
+      </c>
+      <c r="D59" s="11">
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>44339</v>
+        <v>44222</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="10">
-        <v>100</v>
+        <v>18</v>
+      </c>
+      <c r="D60" s="11">
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>44339</v>
+        <v>44222</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="6">
-        <v>73.8</v>
+        <v>32</v>
+      </c>
+      <c r="D61" s="11">
+        <v>13.8</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>44340</v>
+        <v>44223</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="6">
-        <v>399</v>
+        <v>12</v>
+      </c>
+      <c r="D62" s="10">
+        <v>6.16</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>44343</v>
+        <v>44223</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="6">
-        <v>27.3</v>
+        <v>32</v>
+      </c>
+      <c r="D63" s="11">
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>44344</v>
+        <v>44223</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" s="6">
-        <v>399</v>
+        <v>29</v>
+      </c>
+      <c r="D64" s="11">
+        <v>1873.23</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>44346</v>
+        <v>44224</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D65" s="6">
-        <v>66.790000000000006</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>44356</v>
+        <v>44224</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D66" s="6">
-        <v>52.9</v>
+        <v>50.97</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>44358</v>
+        <v>44227</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>3</v>
@@ -1648,138 +1645,132 @@
         <v>13</v>
       </c>
       <c r="D67" s="10">
-        <v>80</v>
+        <v>151.41</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>44359</v>
+        <v>44227</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D68" s="6">
-        <v>9.9</v>
+        <v>15.32</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>44363</v>
+        <v>44228</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D69" s="6">
-        <v>34.69</v>
+        <v>14</v>
+      </c>
+      <c r="D69" s="11">
+        <v>69.8</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>44364</v>
+        <v>44228</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D70" s="6">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="D70" s="11">
+        <v>27.47</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>44365</v>
+        <v>44229</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="10">
-        <v>291.48</v>
+        <v>28</v>
+      </c>
+      <c r="D71" s="11">
+        <v>8.15</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>44367</v>
+        <v>44231</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="10">
-        <v>80</v>
+        <v>18</v>
+      </c>
+      <c r="D72" s="11">
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>44368</v>
+        <v>44231</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73" s="6">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="D73" s="11">
+        <v>6.5</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>44368</v>
+        <v>44235</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" s="6">
-        <v>133</v>
+        <v>14</v>
+      </c>
+      <c r="D74" s="11">
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>44369</v>
+        <v>44235</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75" s="6">
-        <v>45.76</v>
+        <v>34</v>
+      </c>
+      <c r="D75" s="11">
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>44376</v>
+        <v>44237</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="10">
-        <v>80</v>
+        <v>18</v>
+      </c>
+      <c r="D76" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>44381</v>
+        <v>44238</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>3</v>
@@ -1788,157 +1779,160 @@
         <v>13</v>
       </c>
       <c r="D77" s="10">
-        <v>80</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>44382</v>
+        <v>44238</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D78" s="6">
-        <v>68.69</v>
+        <v>18</v>
+      </c>
+      <c r="D78" s="11">
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>44385</v>
+        <v>44238</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D79" s="10">
-        <v>80</v>
+        <v>14</v>
+      </c>
+      <c r="D79" s="11">
+        <v>99.01</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>44413</v>
+        <v>44238</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D80" s="6">
-        <v>68.69</v>
+        <v>5</v>
+      </c>
+      <c r="D80" s="11">
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>44168</v>
+        <v>44239</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D81" s="6">
-        <v>75</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>44169</v>
+        <v>44244</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D82" s="6">
-        <v>200.93</v>
+        <v>13</v>
+      </c>
+      <c r="D82" s="11">
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>44167</v>
+        <v>44244</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D83" s="6">
-        <v>8.15</v>
+        <v>18</v>
+      </c>
+      <c r="D83" s="11">
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>44172</v>
+        <v>44244</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D84" s="6">
-        <v>100</v>
+        <v>5</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D84" s="11">
+        <v>177.81</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>44172</v>
+        <v>44244</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D85" s="6">
-        <v>61</v>
+        <v>32</v>
+      </c>
+      <c r="D85" s="11">
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>44173</v>
+        <v>44246</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D86" s="6">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D86" s="11">
+        <v>44.07</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>44174</v>
+        <v>44246</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" s="6">
-        <v>80</v>
+        <v>14</v>
+      </c>
+      <c r="D87" s="11">
+        <v>77.900000000000006</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>44176</v>
+        <v>44247</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" s="6">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="D88" s="10">
+        <v>291.48</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>44179</v>
+        <v>44247</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>3</v>
@@ -1946,203 +1940,203 @@
       <c r="C89" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D89" s="6">
-        <v>75</v>
+      <c r="D89" s="10">
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>44181</v>
+        <v>44249</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D90" s="6">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D90" s="11">
+        <v>10.34</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>44183</v>
+        <v>44249</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D91" s="6">
-        <v>3439.19</v>
+        <v>25</v>
+      </c>
+      <c r="D91" s="11">
+        <v>51.29</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>44186</v>
+        <v>44249</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D92" s="6">
-        <v>70</v>
+        <v>32</v>
+      </c>
+      <c r="D92" s="11">
+        <v>23.79</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>44186</v>
+        <v>44249</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D93" s="6">
-        <v>246.64</v>
+        <v>14</v>
+      </c>
+      <c r="D93" s="11">
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>44186</v>
+        <v>44250</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D94" s="6">
-        <v>27.7</v>
+        <v>33.909999999999997</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>44186</v>
+        <v>44252</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D95" s="6">
-        <v>48.9</v>
+        <v>13</v>
+      </c>
+      <c r="D95" s="10">
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>44193</v>
+        <v>44252</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D96" s="6">
-        <v>48.8</v>
+        <v>55.8</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>44193</v>
+        <v>44253</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D97" s="6">
-        <v>291.83999999999997</v>
+        <v>29</v>
+      </c>
+      <c r="D97" s="11">
+        <v>2121.6999999999998</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
-        <v>44194</v>
+        <v>44254</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D98" s="11">
-        <v>50</v>
+        <v>4</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="10">
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>44200</v>
+        <v>44254</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D99" s="11">
-        <v>59.67</v>
+        <v>14</v>
+      </c>
+      <c r="D99" s="10">
+        <v>106.32</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
-        <v>44200</v>
+        <v>44256</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D100" s="11">
-        <v>15.41</v>
+        <v>14</v>
+      </c>
+      <c r="D100" s="6">
+        <v>28.7</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
-        <v>44200</v>
+        <v>44256</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D101" s="11">
-        <v>32.03</v>
+        <v>25</v>
+      </c>
+      <c r="D101" s="6">
+        <v>342.12</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
-        <v>44200</v>
+        <v>44257</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D102" s="11">
-        <v>9</v>
+        <v>28</v>
+      </c>
+      <c r="D102" s="6">
+        <v>8.15</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
-        <v>44201</v>
+        <v>44258</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D103" s="11">
-        <v>8.15</v>
+        <v>13</v>
+      </c>
+      <c r="D103" s="10">
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
-        <v>44204</v>
+        <v>44260</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>5</v>
@@ -2150,55 +2144,55 @@
       <c r="C104" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D104" s="11">
-        <v>29</v>
+      <c r="D104" s="6">
+        <v>27</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
-        <v>44207</v>
+        <v>44260</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D105" s="11">
-        <v>15</v>
+        <v>34</v>
+      </c>
+      <c r="D105" s="6">
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
-        <v>44207</v>
+        <v>44260</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D106" s="11">
-        <v>31.23</v>
+        <v>14</v>
+      </c>
+      <c r="D106" s="6">
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
-        <v>44207</v>
+        <v>44263</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D107" s="11">
-        <v>75.3</v>
+        <v>13</v>
+      </c>
+      <c r="D107" s="10">
+        <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
-        <v>44207</v>
+        <v>44263</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>5</v>
@@ -2206,519 +2200,1720 @@
       <c r="C108" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D108" s="11">
-        <v>103.4</v>
+      <c r="D108" s="6">
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
-        <v>44210</v>
+        <v>44267</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D109" s="11">
-        <v>38.25</v>
+        <v>16</v>
+      </c>
+      <c r="D109" s="6">
+        <v>9.9</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
-        <v>44210</v>
+        <v>44270</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D110" s="11">
-        <v>21.69</v>
+        <v>32</v>
+      </c>
+      <c r="D110" s="6">
+        <v>3.89</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
-        <v>44214</v>
+        <v>44270</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D111" s="11">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="D111" s="6">
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
-        <v>44214</v>
+        <v>44274</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D112" s="11">
-        <v>46.9</v>
+        <v>25</v>
+      </c>
+      <c r="D112" s="6">
+        <v>453.17</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
-        <v>44214</v>
+        <v>44275</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D113" s="11">
-        <v>18.5</v>
+        <v>12</v>
+      </c>
+      <c r="D113" s="10">
+        <v>291.48</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
-        <v>44214</v>
+        <v>44276</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D114" s="11">
-        <v>349.11</v>
+        <v>13</v>
+      </c>
+      <c r="D114" s="10">
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
-        <v>44215</v>
+        <v>44276</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" s="11">
-        <v>36.9</v>
+        <v>20</v>
+      </c>
+      <c r="D115" s="6">
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
-        <v>44218</v>
+        <v>44277</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D116" s="11">
-        <v>42.27</v>
+        <v>25</v>
+      </c>
+      <c r="D116" s="6">
+        <v>51.32</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
-        <v>44218</v>
+        <v>44277</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D117" s="11">
-        <v>175.4</v>
+        <v>14</v>
+      </c>
+      <c r="D117" s="6">
+        <v>81.900000000000006</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
-        <v>44218</v>
+        <v>44279</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D118" s="11">
-        <v>1096.74</v>
+        <v>19</v>
+      </c>
+      <c r="D118" s="6">
+        <v>75.180000000000007</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
-        <v>44221</v>
+        <v>44280</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D119" s="11">
-        <v>23.8</v>
+        <v>13</v>
+      </c>
+      <c r="D119" s="10">
+        <v>80</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
-        <v>44221</v>
+        <v>44281</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D120" s="11">
-        <v>392.14</v>
+        <v>14</v>
+      </c>
+      <c r="D120" s="6">
+        <v>70.8</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
-        <v>44221</v>
+        <v>44281</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D121" s="11">
-        <v>2.0299999999999998</v>
+        <v>29</v>
+      </c>
+      <c r="D121" s="6">
+        <v>2121.6999999999998</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
-        <v>44222</v>
+        <v>44284</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D122" s="11">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="D122" s="6">
+        <v>294.01</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
-        <v>44222</v>
+        <v>44284</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D123" s="11">
-        <v>13.8</v>
+        <v>5</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" s="6">
+        <v>3.5</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
-        <v>44223</v>
+        <v>44286</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D124" s="11">
-        <v>14</v>
+      <c r="C124" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D124" s="6">
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
-        <v>44223</v>
+        <v>44287</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D125" s="11">
-        <v>1873.23</v>
+        <v>13</v>
+      </c>
+      <c r="D125" s="10">
+        <v>80</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
-        <v>44228</v>
+        <v>44287</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D126" s="11">
-        <v>69.8</v>
+        <v>30</v>
+      </c>
+      <c r="D126" s="6">
+        <v>9.99</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
-        <v>44228</v>
+        <v>44287</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D127" s="11">
-        <v>27.47</v>
+        <v>5</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" s="6">
+        <v>514.70000000000005</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
-        <v>44229</v>
+        <v>44291</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D128" s="11">
-        <v>8.15</v>
+        <v>30</v>
+      </c>
+      <c r="D128" s="6">
+        <v>19</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
-        <v>44231</v>
+        <v>44291</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D129" s="11">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="D129" s="6">
+        <v>34.69</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
-        <v>44231</v>
+        <v>44291</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D130" s="11">
-        <v>6.5</v>
+        <v>6</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D130" s="6">
+        <v>34.26</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
-        <v>44235</v>
+        <v>44291</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D131" s="11">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D131" s="6">
+        <v>65</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
-        <v>44235</v>
+        <v>44291</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D132" s="11">
-        <v>74</v>
+        <v>28</v>
+      </c>
+      <c r="D132" s="6">
+        <v>8.15</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
-        <v>44238</v>
+        <v>44293</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C133" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D133" s="6">
         <v>18</v>
-      </c>
-      <c r="D133" s="11">
-        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
-        <v>44238</v>
+        <v>44295</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D134" s="11">
-        <v>99.01</v>
+        <v>13</v>
+      </c>
+      <c r="D134" s="10">
+        <v>90</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
-        <v>44238</v>
+        <v>44298</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D135" s="11">
-        <v>130</v>
+        <v>2</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D135" s="6">
+        <v>9.9</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
-        <v>44244</v>
+        <v>44298</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D136" s="11">
-        <v>80</v>
+        <v>25</v>
+      </c>
+      <c r="D136" s="6">
+        <v>69.97</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
-        <v>44244</v>
+        <v>44298</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D137" s="11">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="D137" s="6">
+        <v>51</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
-        <v>44244</v>
+        <v>44302</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D138" s="11">
-        <v>177.81</v>
+        <v>14</v>
+      </c>
+      <c r="D138" s="6">
+        <v>24</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
-        <v>44244</v>
+        <v>44305</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D139" s="11">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D139" s="6">
+        <v>50</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
-        <v>44246</v>
+        <v>44305</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D140" s="11">
-        <v>44.07</v>
+        <v>14</v>
+      </c>
+      <c r="D140" s="6">
+        <v>30.5</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
-        <v>44246</v>
+        <v>44305</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D141" s="11">
-        <v>77.900000000000006</v>
+        <v>25</v>
+      </c>
+      <c r="D141" s="6">
+        <v>406.46</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
-        <v>44249</v>
+        <v>44305</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D142" s="11">
-        <v>10.34</v>
+        <v>34</v>
+      </c>
+      <c r="D142" s="6">
+        <v>40</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
-        <v>44249</v>
+        <v>44306</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D143" s="11">
-        <v>51.29</v>
+        <v>12</v>
+      </c>
+      <c r="D143" s="10">
+        <v>291.48</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
-        <v>44249</v>
+        <v>44308</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D144" s="11">
-        <v>23.79</v>
+        <v>3</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D144" s="10">
+        <v>85</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
-        <v>44249</v>
+        <v>44309</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D145" s="11">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="D145" s="6">
+        <v>262.52999999999997</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
-        <v>44253</v>
+        <v>44312</v>
       </c>
       <c r="B146" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="6">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D147" s="6">
+        <v>39.17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D148" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="6">
+        <v>32.64</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D150" s="6">
+        <v>169.85</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D151" s="6">
+        <v>339.66</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D152" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153" s="6">
+        <v>89.99</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" s="6">
+        <v>77.8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D155" s="6">
+        <v>89.8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D156" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D157" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D158" s="6">
+        <v>87.58</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D159" s="6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D160" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D161" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D162" s="6">
+        <v>11.98</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D163" s="6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D164" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" s="1">
+        <v>44324</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D165" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" s="1">
+        <v>44326</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D166" s="6">
+        <v>34.99</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="1">
+        <v>44328</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D167" s="6">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" s="1">
+        <v>44328</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D168" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D169" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="1">
+        <v>44331</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D170" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D171" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D172" s="6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D173" s="6">
+        <v>57.78</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D174" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" s="1">
+        <v>44336</v>
+      </c>
+      <c r="B175" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C175" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D175" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" s="1">
+        <v>44336</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D176" s="6">
+        <v>200.56</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" s="1">
+        <v>44337</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D177" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" s="1">
+        <v>44338</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D178" s="6">
+        <v>214.62</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D179" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D180" s="6">
+        <v>73.8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D181" s="6">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D182" s="6">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D183" s="6">
+        <v>2121.6999999999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D184" s="6">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D185" s="6">
+        <v>66.790000000000006</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" s="1">
+        <v>44347</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D186" s="6">
+        <v>116.99</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" s="1">
+        <v>44347</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D187" s="6">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D188" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D189" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D190" s="6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D191" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D192" s="6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" s="6">
+        <v>54.51</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D194" s="6">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D195" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" s="1">
+        <v>44359</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D196" s="6">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D146" s="11">
-        <v>2121.6999999999998</v>
+      <c r="D197" s="6">
+        <v>42.99</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" s="6">
+        <v>61.9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D199" s="6">
+        <v>34.69</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D200" s="6">
+        <v>12.72</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D201" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D202" s="6">
+        <v>91.41</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D203" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D204" s="10">
+        <v>291.48</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D205" s="6">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D206" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D207" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D208" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D209" s="6">
+        <v>170.1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D210" s="6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D211" s="6">
+        <v>45.76</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" s="1">
+        <v>44372</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D212" s="6">
+        <v>300.33</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D213" s="6">
+        <v>82.8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D214" s="6">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="1">
+        <v>44376</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D215" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="1">
+        <v>44376</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D216" s="6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D217" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D218" s="6">
+        <v>172.32</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="1">
+        <v>44379</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D219" s="6">
+        <v>19.98</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="1">
+        <v>44379</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D220" s="6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="1">
+        <v>44380</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D221" s="6">
+        <v>11.86</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="1">
+        <v>44380</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D222" s="6">
+        <v>63.25</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="1">
+        <v>44380</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D223" s="6">
+        <v>425.46</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D224" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D225" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" s="1">
+        <v>44382</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D226" s="6">
+        <v>68.69</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="1">
+        <v>44385</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D227" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" s="1">
+        <v>44385</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D228" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="1">
+        <v>44385</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D229" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" s="1">
+        <v>44385</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D230" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" s="1">
+        <v>44386</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D231" s="6">
+        <v>89.72</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" s="1">
+        <v>44386</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D232" s="6">
+        <v>61.9</v>
       </c>
     </row>
   </sheetData>
@@ -2734,7 +3929,7 @@
           <x14:formula1>
             <xm:f>categorias!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B146</xm:sqref>
+          <xm:sqref>B2:B232</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>